<commit_message>
primera parte producto 3
</commit_message>
<xml_diff>
--- a/05_Entregable 3/previo/Diccionarios/MD_02_Judicatura_CJ 0936 Causas Art 247 corte agosto 2024(1).xlsx
+++ b/05_Entregable 3/previo/Diccionarios/MD_02_Judicatura_CJ 0936 Causas Art 247 corte agosto 2024(1).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\05_Entregable 3\previo\Diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="97">
   <si>
     <t>Elemento</t>
   </si>
@@ -65,18 +65,12 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>Nombre de la variable</t>
-  </si>
-  <si>
     <t>Definición</t>
   </si>
   <si>
     <t>Formato de Datos</t>
   </si>
   <si>
-    <t>Unidad de Medida</t>
-  </si>
-  <si>
     <t>Fuente de Datos</t>
   </si>
   <si>
@@ -285,6 +279,48 @@
   </si>
   <si>
     <t>¿PUEDEN HABER VALORES DIFERENTES A LOS PRESENTES EN LA BASE?</t>
+  </si>
+  <si>
+    <t>Nombre actual</t>
+  </si>
+  <si>
+    <t>Nombre propuesto</t>
+  </si>
+  <si>
+    <t>id_juicio</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>instancia</t>
+  </si>
+  <si>
+    <t>delito_accion</t>
+  </si>
+  <si>
+    <t>estado_causa</t>
+  </si>
+  <si>
+    <t>npro</t>
+  </si>
+  <si>
+    <t>ncan</t>
+  </si>
+  <si>
+    <t>fecha_providencia</t>
+  </si>
+  <si>
+    <t>providencia</t>
+  </si>
+  <si>
+    <t>forma_terminacion</t>
+  </si>
+  <si>
+    <t>fecha_providencia_actividad</t>
+  </si>
+  <si>
+    <t>nombre_providencia_actividad</t>
   </si>
 </sst>
 </file>
@@ -729,64 +765,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -794,7 +830,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -806,16 +842,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -824,71 +861,71 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="9">
         <v>43742</v>
@@ -896,126 +933,126 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1039,64 +1076,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1104,7 +1141,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1116,16 +1153,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1134,71 +1169,71 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="9">
         <v>43754</v>
@@ -1206,178 +1241,178 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>58</v>
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>58</v>
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1401,64 +1436,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1466,7 +1501,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1478,16 +1513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1496,195 +1531,195 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
+      <c r="D8" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" s="9">
         <v>44083</v>
@@ -1692,25 +1727,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>